<commit_message>
fix: Send Telegram notification even when PostgreSQL fails
</commit_message>
<xml_diff>
--- a/input/Axima_price.xlsx
+++ b/input/Axima_price.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanabrosimov/Documents/price_system/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A43BECE-4F16-DD4D-A099-996C4CE73675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14074E56-B8F3-3B4A-A48D-60D3B57A6190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19900" xr2:uid="{930496D4-47D5-5948-AE18-CF9084F698A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="375">
   <si>
     <t>Артикул</t>
   </si>
@@ -1158,6 +1158,9 @@
   </si>
   <si>
     <t>Фломастер капиллярный_WAGO_210-110, шт.</t>
+  </si>
+  <si>
+    <t>Проверка2</t>
   </si>
 </sst>
 </file>
@@ -1695,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A3122B-BE9A-8244-AFA2-6A1FF93A067F}">
-  <dimension ref="A1:R187"/>
+  <dimension ref="A1:R188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="I189" sqref="I189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6927,8 +6930,36 @@
         <v>382</v>
       </c>
     </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A188" s="7">
+        <v>9009009</v>
+      </c>
+      <c r="B188" s="7"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7"/>
+      <c r="F188" s="7"/>
+      <c r="G188" s="7"/>
+      <c r="H188" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="I188" s="7"/>
+      <c r="J188" s="7"/>
+      <c r="K188" s="7"/>
+      <c r="L188" s="7"/>
+      <c r="M188" s="7"/>
+      <c r="N188" s="1">
+        <v>100000</v>
+      </c>
+      <c r="O188" s="2"/>
+      <c r="P188" s="2"/>
+      <c r="Q188" s="2"/>
+      <c r="R188" s="3">
+        <v>382</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="373">
+  <mergeCells count="375">
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="H5:M5"/>
     <mergeCell ref="A1:G4"/>
@@ -7292,6 +7323,8 @@
     <mergeCell ref="H178:M178"/>
     <mergeCell ref="A179:G179"/>
     <mergeCell ref="H179:M179"/>
+    <mergeCell ref="A188:G188"/>
+    <mergeCell ref="H188:M188"/>
     <mergeCell ref="A187:G187"/>
     <mergeCell ref="H187:M187"/>
     <mergeCell ref="A185:G185"/>
@@ -7304,5 +7337,6 @@
     <mergeCell ref="H184:M184"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Add concurrency to cancel previous builds when new one starts
</commit_message>
<xml_diff>
--- a/input/Axima_price.xlsx
+++ b/input/Axima_price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanabrosimov/Documents/price_system/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14074E56-B8F3-3B4A-A48D-60D3B57A6190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037C333C-FE2C-6D4A-A55E-80F51F80539E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="19900" xr2:uid="{930496D4-47D5-5948-AE18-CF9084F698A8}"/>
   </bookViews>
@@ -1160,7 +1160,7 @@
     <t>Фломастер капиллярный_WAGO_210-110, шт.</t>
   </si>
   <si>
-    <t>Проверка2</t>
+    <t>Проверка3123123 хуеверкатоп</t>
   </si>
 </sst>
 </file>
@@ -1701,7 +1701,7 @@
   <dimension ref="A1:R188"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
-      <selection activeCell="I189" sqref="I189"/>
+      <selection activeCell="H189" sqref="H189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6960,71 +6960,302 @@
     </row>
   </sheetData>
   <mergeCells count="375">
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="A1:G4"/>
-    <mergeCell ref="H1:M4"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="N1:N4"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="H8:M8"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="H17:M17"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="H12:M12"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="H13:M13"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="A23:G23"/>
-    <mergeCell ref="H23:M23"/>
-    <mergeCell ref="A18:G18"/>
-    <mergeCell ref="H18:M18"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="H19:M19"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="H28:M28"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="A25:G25"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="H26:M26"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="H31:M31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="H32:M32"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="H33:M33"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="H29:M29"/>
-    <mergeCell ref="A30:G30"/>
-    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="A188:G188"/>
+    <mergeCell ref="H188:M188"/>
+    <mergeCell ref="A187:G187"/>
+    <mergeCell ref="H187:M187"/>
+    <mergeCell ref="A185:G185"/>
+    <mergeCell ref="H185:M185"/>
+    <mergeCell ref="A186:G186"/>
+    <mergeCell ref="H186:M186"/>
+    <mergeCell ref="A183:G183"/>
+    <mergeCell ref="H183:M183"/>
+    <mergeCell ref="A184:G184"/>
+    <mergeCell ref="H184:M184"/>
+    <mergeCell ref="A180:G180"/>
+    <mergeCell ref="H180:M180"/>
+    <mergeCell ref="A181:G181"/>
+    <mergeCell ref="H181:M181"/>
+    <mergeCell ref="A182:G182"/>
+    <mergeCell ref="H182:M182"/>
+    <mergeCell ref="A178:G178"/>
+    <mergeCell ref="H178:M178"/>
+    <mergeCell ref="A179:G179"/>
+    <mergeCell ref="H179:M179"/>
+    <mergeCell ref="A175:G175"/>
+    <mergeCell ref="H175:M175"/>
+    <mergeCell ref="A176:G176"/>
+    <mergeCell ref="H176:M176"/>
+    <mergeCell ref="A177:G177"/>
+    <mergeCell ref="H177:M177"/>
+    <mergeCell ref="A172:G172"/>
+    <mergeCell ref="H172:M172"/>
+    <mergeCell ref="A173:G173"/>
+    <mergeCell ref="H173:M173"/>
+    <mergeCell ref="A174:G174"/>
+    <mergeCell ref="H174:M174"/>
+    <mergeCell ref="A169:G169"/>
+    <mergeCell ref="H169:M169"/>
+    <mergeCell ref="A170:G170"/>
+    <mergeCell ref="H170:M170"/>
+    <mergeCell ref="A171:G171"/>
+    <mergeCell ref="H171:M171"/>
+    <mergeCell ref="A168:G168"/>
+    <mergeCell ref="H168:M168"/>
+    <mergeCell ref="A167:G167"/>
+    <mergeCell ref="H167:M167"/>
+    <mergeCell ref="A164:G164"/>
+    <mergeCell ref="H164:M164"/>
+    <mergeCell ref="A165:G165"/>
+    <mergeCell ref="H165:M165"/>
+    <mergeCell ref="A166:G166"/>
+    <mergeCell ref="H166:M166"/>
+    <mergeCell ref="A161:G161"/>
+    <mergeCell ref="H161:M161"/>
+    <mergeCell ref="A162:G162"/>
+    <mergeCell ref="H162:M162"/>
+    <mergeCell ref="A163:G163"/>
+    <mergeCell ref="H163:M163"/>
+    <mergeCell ref="A158:G158"/>
+    <mergeCell ref="H158:M158"/>
+    <mergeCell ref="A159:G159"/>
+    <mergeCell ref="H159:M159"/>
+    <mergeCell ref="A160:G160"/>
+    <mergeCell ref="H160:M160"/>
+    <mergeCell ref="A156:G156"/>
+    <mergeCell ref="H156:M156"/>
+    <mergeCell ref="A157:G157"/>
+    <mergeCell ref="H157:M157"/>
+    <mergeCell ref="A155:G155"/>
+    <mergeCell ref="H155:M155"/>
+    <mergeCell ref="A152:G152"/>
+    <mergeCell ref="H152:M152"/>
+    <mergeCell ref="A153:G153"/>
+    <mergeCell ref="H153:M153"/>
+    <mergeCell ref="A154:G154"/>
+    <mergeCell ref="H154:M154"/>
+    <mergeCell ref="A149:G149"/>
+    <mergeCell ref="H149:M149"/>
+    <mergeCell ref="A150:G150"/>
+    <mergeCell ref="H150:M150"/>
+    <mergeCell ref="A151:G151"/>
+    <mergeCell ref="H151:M151"/>
+    <mergeCell ref="A148:G148"/>
+    <mergeCell ref="H148:M148"/>
+    <mergeCell ref="A146:G146"/>
+    <mergeCell ref="H146:M146"/>
+    <mergeCell ref="A147:G147"/>
+    <mergeCell ref="H147:M147"/>
+    <mergeCell ref="A143:G143"/>
+    <mergeCell ref="H143:M143"/>
+    <mergeCell ref="A144:G144"/>
+    <mergeCell ref="H144:M144"/>
+    <mergeCell ref="A145:G145"/>
+    <mergeCell ref="H145:M145"/>
+    <mergeCell ref="A140:G140"/>
+    <mergeCell ref="H140:M140"/>
+    <mergeCell ref="A141:G141"/>
+    <mergeCell ref="H141:M141"/>
+    <mergeCell ref="A142:G142"/>
+    <mergeCell ref="H142:M142"/>
+    <mergeCell ref="A139:G139"/>
+    <mergeCell ref="H139:M139"/>
+    <mergeCell ref="A136:G136"/>
+    <mergeCell ref="H136:M136"/>
+    <mergeCell ref="A137:G137"/>
+    <mergeCell ref="H137:M137"/>
+    <mergeCell ref="A138:G138"/>
+    <mergeCell ref="H138:M138"/>
+    <mergeCell ref="A133:G133"/>
+    <mergeCell ref="H133:M133"/>
+    <mergeCell ref="A134:G134"/>
+    <mergeCell ref="H134:M134"/>
+    <mergeCell ref="A135:G135"/>
+    <mergeCell ref="H135:M135"/>
+    <mergeCell ref="A130:G130"/>
+    <mergeCell ref="H130:M130"/>
+    <mergeCell ref="A131:G131"/>
+    <mergeCell ref="H131:M131"/>
+    <mergeCell ref="A132:G132"/>
+    <mergeCell ref="H132:M132"/>
+    <mergeCell ref="A127:G127"/>
+    <mergeCell ref="H127:M127"/>
+    <mergeCell ref="A128:G128"/>
+    <mergeCell ref="H128:M128"/>
+    <mergeCell ref="A129:G129"/>
+    <mergeCell ref="H129:M129"/>
+    <mergeCell ref="A124:G124"/>
+    <mergeCell ref="H124:M124"/>
+    <mergeCell ref="A125:G125"/>
+    <mergeCell ref="H125:M125"/>
+    <mergeCell ref="A126:G126"/>
+    <mergeCell ref="H126:M126"/>
+    <mergeCell ref="A121:G121"/>
+    <mergeCell ref="H121:M121"/>
+    <mergeCell ref="A122:G122"/>
+    <mergeCell ref="H122:M122"/>
+    <mergeCell ref="A123:G123"/>
+    <mergeCell ref="H123:M123"/>
+    <mergeCell ref="A118:G118"/>
+    <mergeCell ref="H118:M118"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="H119:M119"/>
+    <mergeCell ref="A120:G120"/>
+    <mergeCell ref="H120:M120"/>
+    <mergeCell ref="A115:G115"/>
+    <mergeCell ref="H115:M115"/>
+    <mergeCell ref="A116:G116"/>
+    <mergeCell ref="H116:M116"/>
+    <mergeCell ref="A117:G117"/>
+    <mergeCell ref="H117:M117"/>
+    <mergeCell ref="A112:G112"/>
+    <mergeCell ref="H112:M112"/>
+    <mergeCell ref="A113:G113"/>
+    <mergeCell ref="H113:M113"/>
+    <mergeCell ref="A114:G114"/>
+    <mergeCell ref="H114:M114"/>
+    <mergeCell ref="A109:G109"/>
+    <mergeCell ref="H109:M109"/>
+    <mergeCell ref="A110:G110"/>
+    <mergeCell ref="H110:M110"/>
+    <mergeCell ref="A111:G111"/>
+    <mergeCell ref="H111:M111"/>
+    <mergeCell ref="A108:G108"/>
+    <mergeCell ref="H108:M108"/>
+    <mergeCell ref="A106:G106"/>
+    <mergeCell ref="H106:M106"/>
+    <mergeCell ref="A107:G107"/>
+    <mergeCell ref="H107:M107"/>
+    <mergeCell ref="A105:G105"/>
+    <mergeCell ref="H105:M105"/>
+    <mergeCell ref="A104:G104"/>
+    <mergeCell ref="H104:M104"/>
+    <mergeCell ref="A103:G103"/>
+    <mergeCell ref="H103:M103"/>
+    <mergeCell ref="A101:G101"/>
+    <mergeCell ref="H101:M101"/>
+    <mergeCell ref="A102:G102"/>
+    <mergeCell ref="H102:M102"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="H98:M98"/>
+    <mergeCell ref="A99:G99"/>
+    <mergeCell ref="H99:M99"/>
+    <mergeCell ref="A100:G100"/>
+    <mergeCell ref="H100:M100"/>
+    <mergeCell ref="A95:G95"/>
+    <mergeCell ref="H95:M95"/>
+    <mergeCell ref="A96:G96"/>
+    <mergeCell ref="H96:M96"/>
+    <mergeCell ref="A97:G97"/>
+    <mergeCell ref="H97:M97"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="H92:M92"/>
+    <mergeCell ref="A93:G93"/>
+    <mergeCell ref="H93:M93"/>
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="H94:M94"/>
+    <mergeCell ref="A89:G89"/>
+    <mergeCell ref="H89:M89"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="H90:M90"/>
+    <mergeCell ref="A91:G91"/>
+    <mergeCell ref="H91:M91"/>
+    <mergeCell ref="A86:G86"/>
+    <mergeCell ref="H86:M86"/>
+    <mergeCell ref="A87:G87"/>
+    <mergeCell ref="H87:M87"/>
+    <mergeCell ref="A88:G88"/>
+    <mergeCell ref="H88:M88"/>
+    <mergeCell ref="A83:G83"/>
+    <mergeCell ref="H83:M83"/>
+    <mergeCell ref="A84:G84"/>
+    <mergeCell ref="H84:M84"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="H85:M85"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="H80:M80"/>
+    <mergeCell ref="A81:G81"/>
+    <mergeCell ref="H81:M81"/>
+    <mergeCell ref="A82:G82"/>
+    <mergeCell ref="H82:M82"/>
+    <mergeCell ref="A78:G78"/>
+    <mergeCell ref="H78:M78"/>
+    <mergeCell ref="A79:G79"/>
+    <mergeCell ref="H79:M79"/>
+    <mergeCell ref="A77:G77"/>
+    <mergeCell ref="H77:M77"/>
+    <mergeCell ref="A74:G74"/>
+    <mergeCell ref="H74:M74"/>
+    <mergeCell ref="A75:G75"/>
+    <mergeCell ref="H75:M75"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="H76:M76"/>
+    <mergeCell ref="A72:G72"/>
+    <mergeCell ref="H72:M72"/>
+    <mergeCell ref="A73:G73"/>
+    <mergeCell ref="H73:M73"/>
+    <mergeCell ref="A69:G69"/>
+    <mergeCell ref="H69:M69"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="H70:M70"/>
+    <mergeCell ref="A71:G71"/>
+    <mergeCell ref="H71:M71"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="H68:M68"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="H65:M65"/>
+    <mergeCell ref="A66:G66"/>
+    <mergeCell ref="H66:M66"/>
+    <mergeCell ref="A67:G67"/>
+    <mergeCell ref="H67:M67"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="H62:M62"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="H63:M63"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="H64:M64"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="H59:M59"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="H60:M60"/>
+    <mergeCell ref="A61:G61"/>
+    <mergeCell ref="H61:M61"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="H56:M56"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="H57:M57"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="H58:M58"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="H53:M53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="H54:M54"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="H55:M55"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="H50:M50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="H51:M51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="H52:M52"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="H47:M47"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="H48:M48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="H49:M49"/>
+    <mergeCell ref="A44:G44"/>
+    <mergeCell ref="H44:M44"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="H45:M45"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="H46:M46"/>
+    <mergeCell ref="A41:G41"/>
+    <mergeCell ref="H41:M41"/>
+    <mergeCell ref="A42:G42"/>
+    <mergeCell ref="H42:M42"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="H43:M43"/>
     <mergeCell ref="A38:G38"/>
     <mergeCell ref="H38:M38"/>
     <mergeCell ref="A39:G39"/>
@@ -7039,302 +7270,71 @@
     <mergeCell ref="H35:M35"/>
     <mergeCell ref="A36:G36"/>
     <mergeCell ref="H36:M36"/>
-    <mergeCell ref="A44:G44"/>
-    <mergeCell ref="H44:M44"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="H45:M45"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="H46:M46"/>
-    <mergeCell ref="A41:G41"/>
-    <mergeCell ref="H41:M41"/>
-    <mergeCell ref="A42:G42"/>
-    <mergeCell ref="H42:M42"/>
-    <mergeCell ref="A43:G43"/>
-    <mergeCell ref="H43:M43"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="H50:M50"/>
-    <mergeCell ref="A51:G51"/>
-    <mergeCell ref="H51:M51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="H52:M52"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="H47:M47"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="H48:M48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="H49:M49"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="H56:M56"/>
-    <mergeCell ref="A57:G57"/>
-    <mergeCell ref="H57:M57"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="H58:M58"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="H53:M53"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="H54:M54"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="H55:M55"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="H62:M62"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="H63:M63"/>
-    <mergeCell ref="A64:G64"/>
-    <mergeCell ref="H64:M64"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="H59:M59"/>
-    <mergeCell ref="A60:G60"/>
-    <mergeCell ref="H60:M60"/>
-    <mergeCell ref="A61:G61"/>
-    <mergeCell ref="H61:M61"/>
-    <mergeCell ref="A69:G69"/>
-    <mergeCell ref="H69:M69"/>
-    <mergeCell ref="A70:G70"/>
-    <mergeCell ref="H70:M70"/>
-    <mergeCell ref="A71:G71"/>
-    <mergeCell ref="H71:M71"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="H68:M68"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="H65:M65"/>
-    <mergeCell ref="A66:G66"/>
-    <mergeCell ref="H66:M66"/>
-    <mergeCell ref="A67:G67"/>
-    <mergeCell ref="H67:M67"/>
-    <mergeCell ref="A77:G77"/>
-    <mergeCell ref="H77:M77"/>
-    <mergeCell ref="A74:G74"/>
-    <mergeCell ref="H74:M74"/>
-    <mergeCell ref="A75:G75"/>
-    <mergeCell ref="H75:M75"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="H76:M76"/>
-    <mergeCell ref="A72:G72"/>
-    <mergeCell ref="H72:M72"/>
-    <mergeCell ref="A73:G73"/>
-    <mergeCell ref="H73:M73"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="H80:M80"/>
-    <mergeCell ref="A81:G81"/>
-    <mergeCell ref="H81:M81"/>
-    <mergeCell ref="A82:G82"/>
-    <mergeCell ref="H82:M82"/>
-    <mergeCell ref="A78:G78"/>
-    <mergeCell ref="H78:M78"/>
-    <mergeCell ref="A79:G79"/>
-    <mergeCell ref="H79:M79"/>
-    <mergeCell ref="A86:G86"/>
-    <mergeCell ref="H86:M86"/>
-    <mergeCell ref="A87:G87"/>
-    <mergeCell ref="H87:M87"/>
-    <mergeCell ref="A88:G88"/>
-    <mergeCell ref="H88:M88"/>
-    <mergeCell ref="A83:G83"/>
-    <mergeCell ref="H83:M83"/>
-    <mergeCell ref="A84:G84"/>
-    <mergeCell ref="H84:M84"/>
-    <mergeCell ref="A85:G85"/>
-    <mergeCell ref="H85:M85"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="H92:M92"/>
-    <mergeCell ref="A93:G93"/>
-    <mergeCell ref="H93:M93"/>
-    <mergeCell ref="A94:G94"/>
-    <mergeCell ref="H94:M94"/>
-    <mergeCell ref="A89:G89"/>
-    <mergeCell ref="H89:M89"/>
-    <mergeCell ref="A90:G90"/>
-    <mergeCell ref="H90:M90"/>
-    <mergeCell ref="A91:G91"/>
-    <mergeCell ref="H91:M91"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="H98:M98"/>
-    <mergeCell ref="A99:G99"/>
-    <mergeCell ref="H99:M99"/>
-    <mergeCell ref="A100:G100"/>
-    <mergeCell ref="H100:M100"/>
-    <mergeCell ref="A95:G95"/>
-    <mergeCell ref="H95:M95"/>
-    <mergeCell ref="A96:G96"/>
-    <mergeCell ref="H96:M96"/>
-    <mergeCell ref="A97:G97"/>
-    <mergeCell ref="H97:M97"/>
-    <mergeCell ref="A105:G105"/>
-    <mergeCell ref="H105:M105"/>
-    <mergeCell ref="A104:G104"/>
-    <mergeCell ref="H104:M104"/>
-    <mergeCell ref="A103:G103"/>
-    <mergeCell ref="H103:M103"/>
-    <mergeCell ref="A101:G101"/>
-    <mergeCell ref="H101:M101"/>
-    <mergeCell ref="A102:G102"/>
-    <mergeCell ref="H102:M102"/>
-    <mergeCell ref="A109:G109"/>
-    <mergeCell ref="H109:M109"/>
-    <mergeCell ref="A110:G110"/>
-    <mergeCell ref="H110:M110"/>
-    <mergeCell ref="A111:G111"/>
-    <mergeCell ref="H111:M111"/>
-    <mergeCell ref="A108:G108"/>
-    <mergeCell ref="H108:M108"/>
-    <mergeCell ref="A106:G106"/>
-    <mergeCell ref="H106:M106"/>
-    <mergeCell ref="A107:G107"/>
-    <mergeCell ref="H107:M107"/>
-    <mergeCell ref="A115:G115"/>
-    <mergeCell ref="H115:M115"/>
-    <mergeCell ref="A116:G116"/>
-    <mergeCell ref="H116:M116"/>
-    <mergeCell ref="A117:G117"/>
-    <mergeCell ref="H117:M117"/>
-    <mergeCell ref="A112:G112"/>
-    <mergeCell ref="H112:M112"/>
-    <mergeCell ref="A113:G113"/>
-    <mergeCell ref="H113:M113"/>
-    <mergeCell ref="A114:G114"/>
-    <mergeCell ref="H114:M114"/>
-    <mergeCell ref="A121:G121"/>
-    <mergeCell ref="H121:M121"/>
-    <mergeCell ref="A122:G122"/>
-    <mergeCell ref="H122:M122"/>
-    <mergeCell ref="A123:G123"/>
-    <mergeCell ref="H123:M123"/>
-    <mergeCell ref="A118:G118"/>
-    <mergeCell ref="H118:M118"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="H119:M119"/>
-    <mergeCell ref="A120:G120"/>
-    <mergeCell ref="H120:M120"/>
-    <mergeCell ref="A127:G127"/>
-    <mergeCell ref="H127:M127"/>
-    <mergeCell ref="A128:G128"/>
-    <mergeCell ref="H128:M128"/>
-    <mergeCell ref="A129:G129"/>
-    <mergeCell ref="H129:M129"/>
-    <mergeCell ref="A124:G124"/>
-    <mergeCell ref="H124:M124"/>
-    <mergeCell ref="A125:G125"/>
-    <mergeCell ref="H125:M125"/>
-    <mergeCell ref="A126:G126"/>
-    <mergeCell ref="H126:M126"/>
-    <mergeCell ref="A133:G133"/>
-    <mergeCell ref="H133:M133"/>
-    <mergeCell ref="A134:G134"/>
-    <mergeCell ref="H134:M134"/>
-    <mergeCell ref="A135:G135"/>
-    <mergeCell ref="H135:M135"/>
-    <mergeCell ref="A130:G130"/>
-    <mergeCell ref="H130:M130"/>
-    <mergeCell ref="A131:G131"/>
-    <mergeCell ref="H131:M131"/>
-    <mergeCell ref="A132:G132"/>
-    <mergeCell ref="H132:M132"/>
-    <mergeCell ref="A140:G140"/>
-    <mergeCell ref="H140:M140"/>
-    <mergeCell ref="A141:G141"/>
-    <mergeCell ref="H141:M141"/>
-    <mergeCell ref="A142:G142"/>
-    <mergeCell ref="H142:M142"/>
-    <mergeCell ref="A139:G139"/>
-    <mergeCell ref="H139:M139"/>
-    <mergeCell ref="A136:G136"/>
-    <mergeCell ref="H136:M136"/>
-    <mergeCell ref="A137:G137"/>
-    <mergeCell ref="H137:M137"/>
-    <mergeCell ref="A138:G138"/>
-    <mergeCell ref="H138:M138"/>
-    <mergeCell ref="A148:G148"/>
-    <mergeCell ref="H148:M148"/>
-    <mergeCell ref="A146:G146"/>
-    <mergeCell ref="H146:M146"/>
-    <mergeCell ref="A147:G147"/>
-    <mergeCell ref="H147:M147"/>
-    <mergeCell ref="A143:G143"/>
-    <mergeCell ref="H143:M143"/>
-    <mergeCell ref="A144:G144"/>
-    <mergeCell ref="H144:M144"/>
-    <mergeCell ref="A145:G145"/>
-    <mergeCell ref="H145:M145"/>
-    <mergeCell ref="A155:G155"/>
-    <mergeCell ref="H155:M155"/>
-    <mergeCell ref="A152:G152"/>
-    <mergeCell ref="H152:M152"/>
-    <mergeCell ref="A153:G153"/>
-    <mergeCell ref="H153:M153"/>
-    <mergeCell ref="A154:G154"/>
-    <mergeCell ref="H154:M154"/>
-    <mergeCell ref="A149:G149"/>
-    <mergeCell ref="H149:M149"/>
-    <mergeCell ref="A150:G150"/>
-    <mergeCell ref="H150:M150"/>
-    <mergeCell ref="A151:G151"/>
-    <mergeCell ref="H151:M151"/>
-    <mergeCell ref="A158:G158"/>
-    <mergeCell ref="H158:M158"/>
-    <mergeCell ref="A159:G159"/>
-    <mergeCell ref="H159:M159"/>
-    <mergeCell ref="A160:G160"/>
-    <mergeCell ref="H160:M160"/>
-    <mergeCell ref="A156:G156"/>
-    <mergeCell ref="H156:M156"/>
-    <mergeCell ref="A157:G157"/>
-    <mergeCell ref="H157:M157"/>
-    <mergeCell ref="A164:G164"/>
-    <mergeCell ref="H164:M164"/>
-    <mergeCell ref="A165:G165"/>
-    <mergeCell ref="H165:M165"/>
-    <mergeCell ref="A166:G166"/>
-    <mergeCell ref="H166:M166"/>
-    <mergeCell ref="A161:G161"/>
-    <mergeCell ref="H161:M161"/>
-    <mergeCell ref="A162:G162"/>
-    <mergeCell ref="H162:M162"/>
-    <mergeCell ref="A163:G163"/>
-    <mergeCell ref="H163:M163"/>
-    <mergeCell ref="A169:G169"/>
-    <mergeCell ref="H169:M169"/>
-    <mergeCell ref="A170:G170"/>
-    <mergeCell ref="H170:M170"/>
-    <mergeCell ref="A171:G171"/>
-    <mergeCell ref="H171:M171"/>
-    <mergeCell ref="A168:G168"/>
-    <mergeCell ref="H168:M168"/>
-    <mergeCell ref="A167:G167"/>
-    <mergeCell ref="H167:M167"/>
-    <mergeCell ref="A175:G175"/>
-    <mergeCell ref="H175:M175"/>
-    <mergeCell ref="A176:G176"/>
-    <mergeCell ref="H176:M176"/>
-    <mergeCell ref="A177:G177"/>
-    <mergeCell ref="H177:M177"/>
-    <mergeCell ref="A172:G172"/>
-    <mergeCell ref="H172:M172"/>
-    <mergeCell ref="A173:G173"/>
-    <mergeCell ref="H173:M173"/>
-    <mergeCell ref="A174:G174"/>
-    <mergeCell ref="H174:M174"/>
-    <mergeCell ref="A180:G180"/>
-    <mergeCell ref="H180:M180"/>
-    <mergeCell ref="A181:G181"/>
-    <mergeCell ref="H181:M181"/>
-    <mergeCell ref="A182:G182"/>
-    <mergeCell ref="H182:M182"/>
-    <mergeCell ref="A178:G178"/>
-    <mergeCell ref="H178:M178"/>
-    <mergeCell ref="A179:G179"/>
-    <mergeCell ref="H179:M179"/>
-    <mergeCell ref="A188:G188"/>
-    <mergeCell ref="H188:M188"/>
-    <mergeCell ref="A187:G187"/>
-    <mergeCell ref="H187:M187"/>
-    <mergeCell ref="A185:G185"/>
-    <mergeCell ref="H185:M185"/>
-    <mergeCell ref="A186:G186"/>
-    <mergeCell ref="H186:M186"/>
-    <mergeCell ref="A183:G183"/>
-    <mergeCell ref="H183:M183"/>
-    <mergeCell ref="A184:G184"/>
-    <mergeCell ref="H184:M184"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="H31:M31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="H32:M32"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="H33:M33"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="H29:M29"/>
+    <mergeCell ref="A30:G30"/>
+    <mergeCell ref="H30:M30"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="H28:M28"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="H23:M23"/>
+    <mergeCell ref="A18:G18"/>
+    <mergeCell ref="H18:M18"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="H19:M19"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="H17:M17"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="H12:M12"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="H13:M13"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="H7:M7"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="H8:M8"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="A1:G4"/>
+    <mergeCell ref="H1:M4"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="N1:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>